<commit_message>
Get daily reddit data: Tue May 21 08:08:50 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_26.xlsx
+++ b/data/2024_05_26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C457"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5551,6 +5551,2658 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1cx1xiv</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Pink french ❤️</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q50r8b1jcq1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1cx1ida</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Hey Fwends🦦</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rb4826ji7q1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1cx1hpa</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>problem</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cx1hpa/problem/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1cx1gaz</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>My 1😌</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58fzdnhs6q1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1cwx0cm</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Weak nails</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwx0cm</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1cwynul</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>DND gel and pitting</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kkw3irvap1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1cwzp57</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Press Ons</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cwzp57/press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1cx0rr3</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just finished a nailset  for the customer's graduation photoshoot / press-on try on </t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ops7j4eyp1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1cx0egb</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Wedding dip nails (swipe for non-cursed pose)</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cx0egb</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1cx07sw</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Some favorite nail sets that I’ve done this year! 💅🏼</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cx07sw</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1cwzoh5</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail shop receptionist </t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cwzoh5/nail_shop_receptionist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1cwzn0s</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>My claws!</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4fehv38lp1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1cwyqyf</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Healthy cuticles?</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bapo4ayrbp1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1cwyit2</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>I did my own dipped powder/gel manicure. What do you think?</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/78zky01g9p1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1cwyelo</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>How can I fix my nail shape?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwyelo</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1cwxvob</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>My first attempt at water marbling!</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwxvob</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1cww93k</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lf6vcb12oo1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1cwvyzn</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mavala Buenos Aires </t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/grqo0clklo1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1cwvv2k</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>I’m obsessed!</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7ult7nkko1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1cwvqjt</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>M&amp;N Indie Polish - Blue Weevil</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwvqjt</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1cwumic</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Asking for Help from the Builder Nail Gel Experts!</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cwumic/asking_for_help_from_the_builder_nail_gel_experts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1cwvjhb</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Some gel x nails I did over the past few months 💕</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwvjhb</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1cwv83f</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Koi fish nails</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwv83f</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1cwunjm</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Natural Nails</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwunjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1cwu8z4</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My set for the next few days! ♥︎ </t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwu8z4</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1cwu0n5</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Accidentally did end portal nails and I love them </t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwu0n5</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1cwtvb9</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">super dry cuticles </t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cwtvb9/super_dry_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1cwtqhp</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>$2 shein press ons + gel top coat = 💅🏽🔥</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwtqhp</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1cwsnge</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>been a while since my last post but here’s my bare natural nails 💅</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwsnge</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1cwsio0</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail tech did an amazing job once again </t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwsio0</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1cws5ak</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Which nail glue for press-one</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cws5ak</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1cwr2t0</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Bitten by Sinful Colors</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fec6fy5xgn1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1cwqxd5</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>OPI Dutch Tulips</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7cavplurfn1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1cwqdd9</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Went longer than usual, freshly done :)</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwqdd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1cwq7df</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>What's that called? And where can I find it?</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cwq7df/whats_that_called_and_where_can_i_find_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1cwpz3x</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer vibes </t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwpz3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1cwpw1a</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any tips to make my natural nails look better? Shapes or file techniques? </t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwpw1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1cwpvbg</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Sparkly nude-ish nails before I cut them all super short bc of a break :(</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cubujc9v7n1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1cwp6a0</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Acrylic removal questions.</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cwp6a0/acrylic_removal_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1cwp1wa</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Best Option for Teens (full set)</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cwp1wa/best_option_for_teens_full_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1cwov0t</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>picnic vibes 🧺🍒⭐️</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rm7c89li0n1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1cwooj1</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Metallic vibes with foils and mirror chrome powders. </t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nttkpgd8zm1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1cwojkv</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Did my own gel sparkly French mani 🥰</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwojkv</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1cvxxle</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Gel polish question</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cvxxle/gel_polish_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1cw0z29</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Repeat After Me..</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cw0z29</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1cw26t0</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>First time going to a nail salon</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cw26t0/first_time_going_to_a_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1cw363e</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Accidentally ripped part of nail from Press On removal (not through bed). How can I "fill" my dent and protect the nail?</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9tppp0anbh1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1cw5hx2</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Those of you who keep your nails looking pretty for the long term… how do you do it?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cw5hx2/those_of_you_who_keep_your_nails_looking_pretty/</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1cw5rxe</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>What are the weird lines?</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sbsyn3yg0i1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1cw7br4</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Latex free nail salons?</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cw7br4/latex_free_nail_salons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1cw9md8</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Design perspective: Do you think keeping the thumbnail shorter looks odd?</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cw9md8/design_perspective_do_you_think_keeping_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1cwd5ml</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Builder gel removal? </t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cwd5ml/builder_gel_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1cwf81u</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Dip at home-what do I need and need to know?</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cwf81u/dip_at_homewhat_do_i_need_and_need_to_know/</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1cwhzci</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Latest press ons!</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwhzci</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1cwkhce</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>do press ons permanently damage your nails?</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cwkhce/do_press_ons_permanently_damage_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1cwmth4</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Mooncat Sabertooth 🦕✨🩵</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwmth4</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1cwniog</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>My nail tech is the best</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/86fcd4eoqm1d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1cwnchk</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>I love my independent nail tech!</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwnchk</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1cwn7md</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Snail Inspo</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ki5ux2uhom1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1cwna4e</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>My first set</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwna4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1cwmr64</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>They look so delicate 🌹</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5gsyhb4lm1d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1cwm2gi</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Acrylic vs Builder Gel</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cwm2gi/acrylic_vs_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1cwlr4w</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Ombre 🩷🤍 what do you think?</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/en2fut6rdm1d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1cwl6vo</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>My first non-lumpy freehand polygel application! 🥲</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6o828gl9m1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1cwl1y1</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Did my own gel x nails for the first time!🥰</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6prffx2j8m1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1cwjski</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Everytime I paint my nails they get messed up</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cwjski/everytime_i_paint_my_nails_they_get_messed_up/</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1cwjrp5</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>I’ll be serving tonight &lt;3</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kx0s68oxyl1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1cwjnz6</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Rattlesnake nails</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwjnz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1cwj40s</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel X application question </t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cwj40s/gel_x_application_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1cwitju</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Brittle nail recommendation. Clear polish?</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cwitju/brittle_nail_recommendation_clear_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1cwioyo</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>My nails bend a weird shape?</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwioyo</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1cwim5s</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>come see these beauties🤩🤩🤩🤩🤩🤩🤩🤩🤩</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwim5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1cwilh6</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>I recommend the cat eye effect if you want something bold but subtle</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwilh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1cwiblf</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Butterfly nails 🦋</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7kx766zvnl1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1cwi8t9</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did them myself </t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1qybgknanl1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1cwi3yb</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Marbled nails 🌈 </t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0ue4awbml1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1cwhvbl</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Beginner Nail Tech</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwhvbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1cwhlb5</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Vacation Nails</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwhlb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1cwh1as</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Nails to match a dress for my sister</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwh1as</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1cwgykr</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>I’m in love with this color on me</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/md11aqcgdl1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1cwgqq5</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Advice and Tips</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vv247auobl1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1cwen7x</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Finally! A press on set I don’t have to cut shorter!</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwen7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1cwe3kc</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Mixed 2 packs of left over press ons aaaaand I’m obsessed 💅💅💅</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwe3kc</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1cwdkks</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>I started making press-ons the other week and I need some advice with this set</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j02dzthakk1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1cwd9oa</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Rammstein nails for my sister</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwd9oa</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1cwcjs1</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm so mad </t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xo0h0nbi9k1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1cwce6j</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Cons to living on a small island…</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwce6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1cwc9ba</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>i need to get a photo of these in the sunlight but dang my nail tech killed it</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwc9ba</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1cwc4x4</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first time trying chrome powders </t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwc4x4</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1cx2cj7</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Contacting mooncat</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eyo73vqzhq1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1cx1pmz</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>New set, I’m obsessed!</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cx1pmz</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1cx0v0o</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Second attempt at nail art! Beach nails!</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cx0v0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1cwzuat</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which polishes have the most aesthetic bottles in your opinion? </t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cwzuat/which_polishes_have_the_most_aesthetic_bottles_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1cwy4yg</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>I got my Mooncat order and decided to go with Plankton first</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwy4yg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1cwdnta</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Hozier Tour Nails</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwdnta</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1cwxxbl</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>My first attempt at water marbling!</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwxxbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1cwx8fk</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>obsessed with mooncat’s “queen of the dead” thermal lacquer</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ma5vxlxxwo1d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1cwx8hs</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>New Fancy Gloss super fan 😍 (also featuring judgemental dog)</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwx8hs</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1cwws29</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Help identifying Japanese polish?</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwws29</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1cwvt69</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t xml:space="preserve">M&amp;N Indie Polish - Blue Weevil </t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwvt69</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1cwvrd6</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>I waited a year to finally try this. Atomic Polish Sour Apple Rings</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/csqurbhnjo1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1cwuyvq</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Mermaid Bait to celebrate Mermay! 🧜‍♂️</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwuyvq</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1cwuwhv</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Cirque Colors- You Tart!</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwuwhv</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1cwu6lx</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nail art ideas? </t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwu6lx</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1cwu5nn</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Dangerous Beauty - Vanessa Molina</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/asfvxxyl5o1d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1cwtrlb</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>KBShimmer - Sip Back and Relax</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwtrlb</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1cwtph4</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>AI search on insta is the worst…</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4h8ldgs1o1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1cwtm65</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Tried my hand at nails like Effie Trinket's in the first Hunger Games movie</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwtm65</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1cws5m9</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Strawberry nail art 🍓</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v82ryzt5pn1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1cws5a9</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Talk me down from this purchase!</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/59gtgdh3pn1d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1cwruy3</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Garden Path Lacquers - The World's a Little Blurry (PPU April '24)</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/snsuahswmn1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1cwrrga</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I had my Instagram followers submit drawings of what to do with my nails. I chose this super weird, creepy submission. How'd I do? (swipe for my take) </t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwrrga</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1cwrr3y</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t xml:space="preserve">True life: my thermal is stuck on cold </t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cwrr3y/true_life_my_thermal_is_stuck_on_cold/</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1cwqk1a</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Question about thermals</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cwqk1a/question_about_thermals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1cwq25m</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red, white, and blue polish </t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cwq25m/red_white_and_blue_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1cwpxz0</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Cremes and metallics just look so good together. 😍</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwpxz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1cwpv0o</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>House of Hades for purple lovers</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/orh96h2m7n1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1cwp7au</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>A pop of colour for the summer</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwp7au</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1cwoekb</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>What's your "Hell no!" price point?</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cwoekb/whats_your_hell_no_price_point/</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1cwo5ro</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>a little fruit salad 🍇🍉🍊</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwo5ro</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1cwo2rv</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>My attempt at a holo jelly gradient</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwo2rv</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1cwnar8</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Sailor moon inspired nails</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwnar8</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1cwn5ih</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Help with bendy nails</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwn5ih</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1cwn1sk</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Major shrinkage from Vibrant Scents Fast &amp; Hard, is it my application? </t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cwn1sk/major_shrinkage_from_vibrant_scents_fast_hard_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1cwmuu2</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Taco Bell x ILNP? 🤣</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4alk334vlm1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1cwm8j4</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>If you had to pick JUST ONE, what is your all-time favorite polish?</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cwm8j4/if_you_had_to_pick_just_one_what_is_your_alltime/</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1cwm50l</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>My ball python and my blues 💙</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwm50l</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1cwltpa</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>I know it’s Spring, but I had to get in just one more brown mani….</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vj5edl5bem1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1cwled7</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Glitter taupe ✨</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75lzos66bm1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1cwl507</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Looking for 2 Madam Glam dupes!</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwl507</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1cwkytq</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Staycation by ilnp</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqbxy67v7m1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1cwk3mj</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>First Mooncat order and I'm obsessed with this colour for summer</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okihgpzf1m1d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1cwjy6l</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>I loooove Orly (&amp; ILNP)</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwjy6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1cwjopd</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Shamrock and Roll</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwjopd</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1cwj3c6</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Bees Knees Arcana</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwj3c6</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1cwie7i</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Obsessed with this neon coral color - anyone know a dupe?</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwie7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1cwhk2z</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Help troubleshooting Glisten &amp; Glow topcoat</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/doaye657il1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1cwhf4i</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Shout out to this group</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwhf4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1cwhbl8</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>How often do you palette cleanse your nails?</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cwhbl8/how_often_do_you_palette_cleanse_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1cwh8qn</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>My first indies 😍</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwh8qn</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1cwgph4</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Newbie to the wider world of non-drugstore brands. Can anyone help me find a really good color match to this blue scarf? The color name is 'Mazarine Blue' and it's intensely blue with a purple edge - not quite cobalt but definitely not navy. [stock photo]</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gf6mjquwal1d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1cwf4u6</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Another Mooncat Treachery in Blue Post </t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ooswz5nyk1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1cwbvmb</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cwbvmb/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1cwapvj</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>I've gotten really into magnetic polish lately - this khaki and blue shift really scratches my brain</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwapvj</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1cwxutd</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>My first attempt at water marbling!</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwxutd</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1cwtute</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Cat talking meme | 3D sculpting with carving gel</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwtute</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1cwrmgz</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>My newest gel Nails with nordic runes!</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwrmgz</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1cwr9wu</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Fruit nails 🍓🍇🍒🍊</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwr9wu</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1cwp2qp</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails done for the week </t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtltjl312n1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1cwoxkt</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>I did some practice nailart with pigments</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwoxkt</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1cwn6gr</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Don’t ask why</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwn6gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1cwmgck</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glazed Donut with Sprinkles </t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9rwvx0uim1d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1cwltew</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Some flowers for tge next couple weeks</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b5xegdt8em1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1cwlr8c</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Really enjoying my character art journey!</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwlr8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1cwk2zm</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>An early summer set (IG: juun.yc)</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwk2zm</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1cwgmvl</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Rose Stained Glass</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cwgmvl</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed May 22 08:09:25 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_26.xlsx
+++ b/data/2024_05_26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C457"/>
+  <dimension ref="A1:C612"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8203,6 +8203,2641 @@
         </is>
       </c>
     </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1cxuz0x</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Thank God my bestie has patience this took me forever🥵 (beginner)</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxuz0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1cxun65</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Amazon reviews: “these tips are too sharp ☹️” Me: SOLD</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qt3teztvlx1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1cxulpa</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>This nude shade is always 💖✨</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxulpa</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1cxuklx</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Was I overcharged? An invitation to discuss and a request for comfort</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxuklx</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1cxtqox</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Good? Bad? New to extensions. </t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxtqox</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1cxtg6x</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Green and silver nails 💚🤍</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rwid8if27x1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1cxt0tp</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Tried some cherries! 🍒☀️</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxt0tp</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1cxmnae</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>{PR} Strawberry Nails</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxmnae</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1cxsk2p</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My current set:) </t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxsk2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1cxsief</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>just feel like this isn’t said enough in this chat.</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cxsief/just_feel_like_this_isnt_said_enough_in_this_chat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1cxruvh</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>I regret choosing cuteness over functionality 🥲🤭</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxruvh</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1cxrmr7</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Nails pointing up?</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fy171achmw1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1cxqj8r</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>My first press on 🥺✨</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxqj8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1cxqim5</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Natural nails</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/27rf4qubbw1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1cxq20u</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple &amp; clean </t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kg1li73t6w1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1cxpkgt</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Simply simple, elegant and delicate ✨</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1au540182w1d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1cxpg0z</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Amethyst accent nail 💜</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a6b3tsm31w1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1cxp6ie</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>they are beautiful! I know! salmon!</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3bcn283lyv1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1cxp328</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Spikey flowers</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5thuy8pxv1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1cxo94g</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>tipping</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cxo94g/tipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1cxnf4r</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Progress Pics </t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxnf4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1cxmsrg</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>thoughts?</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxmsrg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1cxmnxr</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>I love the blue nails</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxmnxr</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1cxmn8a</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh mani </t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uuvzvkwkbv1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1cxmm01</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>I love my manicure work</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f4bqk3babv1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1cxmkp3</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Absolutely in love with my new nails</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0eiip86zav1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1cxm6dm</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Help!!</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxm6dm</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1cxm5zg</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Simple &amp; sweet glue-on’s (Olive &amp; June from Target!)</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxm5zg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1cxm3bi</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Wanted to go with a “summer” theme. Idk if it’s summer, but I think they’re cute!</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qpd23evw6v1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1cxli5w</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>🥰🥰🥰🥰</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxli5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1cxlhxl</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yeah, I know they're obnoxious. 😄 </t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7b9sofow1v1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1cxldi5</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Plant Nails</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxldi5</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1cxkcvs</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you like this set? </t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6hrs27ssu1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1cxk1f9</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Butterfly press ons for spring 🦋🦋🦋</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbg2zjyfqu1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1cxjji8</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This colour makes me feel like a pistachio gelato </t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4thnp9omu1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1cxjg0q</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New acrylics set </t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxjg0q</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1cxiwz9</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Peeling.</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cxiwz9/peeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1cxirbr</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Bridgerton watch party nails</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yhu3htlogu1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1cximev</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>First frenchies ever on myself 🥰</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cximev</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1cxhvkj</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Club thumb - Press ons?</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0bkvkw23au1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1cxhvd7</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>New spring set</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxhvd7</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1cxhe9p</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I kinda hate it </t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/78ephf9i6u1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1cxhakw</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>My absolute favorite thing is freshly done cuticles 🥰 even if it makes my grow-out more apparent lol</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxhakw</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1cxh4lf</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Set I did last night for my bestie</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxh4lf</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1cx6gm3</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>New set inspired by my new purse 🍒💖🌸</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cx6gm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1cxbd5k</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Does anyone know where to get a pack of long press ons but in children’s size?</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cxbd5k/does_anyone_know_where_to_get_a_pack_of_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1cxgxe1</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>First time trying sip on myself. Not too mad about it!</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxgxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1cxguel</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Redbull &amp; nails! </t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6cwmicl2u1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1cxgs43</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>So baaaad 😂</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxgs43</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1cxgmb6</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Not sure what to think about this set 😓</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ymhgm71y0u1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1cxgfj5</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Champagne sparkles</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxgfj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1cxg0rz</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>delicate! beautiful! pink!</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6be8hl6kwt1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1cxft02</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm starting, recommendations? </t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8c5fdv0vt1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1cxfiyx</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>i adore my new set 🎀💖</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jiolmll1tt1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1cxfev2</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Loving this color combination 😻🥳</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5uh3z87st1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1cxf0hu</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Found a fix for nail peeling from gel use! </t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cxf0hu/found_a_fix_for_nail_peeling_from_gel_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1cxetmu</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Some nail art designs I’ve done over the past couple months</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxetmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1cxeozy</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Moving soon &amp; no time for Polygel, thought I’d try making some press ons</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxeozy</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1cxeo0k</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I have a question about natural nails!!! </t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cxeo0k/i_have_a_question_about_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1cxedse</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I felt deeply compelled to match my nails to my tamagotchi </t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4w58hlgukt1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1cxebih</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Mixed “gradient”</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oatajvzdkt1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1cxd3ef</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Acrylic Pink Cateye 🎀🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxd3ef</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1cxcskj</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Nailfie time !</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qv2gp7649t1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1cxcihu</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>My newest set 🩷💙</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5fvip607t1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1cxcifg</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>I'm out of the manicurist, I don't like them, I see a lot of construction defects. What do the experts say?</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwu9mltz6t1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1cxchyp</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>I get more compliments when i am wearing press ons than when I get my nails at salon</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxchyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1cxcbtm</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Which nail glue for press-ons ✨</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxcbtm</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1cxc39c</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Update: I think I fixed them!</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/42gj9pkt3t1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1cxbjs9</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my nails today. First attempt at French tips. I know they aren't perfect, but I feel like they good for a first try </t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/in0lckmrzs1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1cxa77w</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Newest set!</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxa77w</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1cxa5mz</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>What do we think ?</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxa5mz</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1cxa5jd</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Flat nail beds?</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxg3j538ps1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1cx9h7d</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Fist time</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aabsucm2ks1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1cx9cbc</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>And so, in the end, I decided to switch to the classics. 💅🏻</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cx9cbc</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1cx9aqj</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Advice on drawing lavender?</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cx9aqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1cx99ni</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>some of the nail art I’ve done for my gf!</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cx99ni</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1cx8yyl</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>PhD graduation nails</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gyc0g11gs1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1cx88jh</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Off white French</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cx88jh</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1cx82bv</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>I was going for CD vibes 💿</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cki8l8kn8s1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1cx7zfl</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Do I have “man” hands?</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cx7zfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1cx7j2f</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>New blue nails!</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cx7j2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1cx78pj</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>I’m joining the press-on revolution. The time and expense of the salon can’t be justified when I can do this at home for less than $15.</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cx78pj</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1cx78l0</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you like this set? </t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ldm3fsio1s1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1cx77p4</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Nudity</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0jahhmh1s1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1cx75bp</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Getting better?</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zt5a7dww0s1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1cx6zrk</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Do you share your nail kit with others? Why or why not?</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cx6zrk/do_you_share_your_nail_kit_with_others_why_or_why/</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1cx6r8a</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>I have a beautiful collection of photos of all the times I had a manicure. I love doing it, do you like it?</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/juj92oucxr1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1cx5ze0</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>What are these ridged/dents in my nails? And why is it like this?</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cx5ze0</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1cx5vci</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Duck nails anyone? </t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cx5vci</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1cx5urn</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cats eye granite something something </t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cx5urn</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1cx4fyp</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>stamping plate is defective orrr?</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cx4fyp/stamping_plate_is_defective_orrr/</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1cx3vzb</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>First time using gel extensions. Not my best but was interesting to try something longer.</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cx3vzb</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1cx2sha</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Why my nails are like this?</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f7dkql0tnq1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1cxu3yh</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>A cashier complimented my nails 🥹</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5zpllwe6fx1d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1cxsxsc</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>at least 3/4 made it 💔💔</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1nx8fbqy0x1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1cxss8w</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>🚫 Color Club Gel Polish!</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cxss8w/color_club_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1cxsmwy</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Sally Hansen, you legend</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxsmwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1cxr8pq</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>First LynBDesigns and I’m in love with the collection</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mk337qviiw1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1cxqw7o</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>May this thermal never die!</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxqw7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1cxqvf8</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Spring brights ✨</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0ghrjdfi9w1d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1cxpggs</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>First time doing gradient</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxpggs</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1cxouco</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>What brands are worth the money?</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cxouco/what_brands_are_worth_the_money/</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1cxoev7</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>2 magnet velvet hack!</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kn18zgahrv1d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1cxmkth</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce Strawberry Nails</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxmkth</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1cxmatx</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Custom Nail Decal Printers?</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cxmatx/custom_nail_decal_printers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1cxlx74</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>First time using Glitter Grabber</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aodeznhf5v1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1cxltnr</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Flower Child lives up to the hype!!</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxltnr</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1cxlmnl</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>🕸️🕸️🕸️</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxlmnl</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1cxl4f4</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>The lacqueristic urge to be simultaneously cute and cursed</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxl4f4</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1cxku46</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Zoya Jordan under sunlight</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/afor52oyvu1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1cxkts4</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>My favorite thermal!</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxkts4</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1cxjyjx</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>European brands for nail polish</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cxjyjx/european_brands_for_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1cxjc7z</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>What color to use for the tips if I want to recreate this look?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x1evplj3lu1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1cxj86x</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Jellies after a dehydrating weekend</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxj86x</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1cxi8ln</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Favorite cuticle scissors under $20</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cxi8ln/favorite_cuticle_scissors_under_20/</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1cxi3tm</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Getting the hang of this!</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f44mw9ptbu1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1cxi2po</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Mooncat - Shroomdom</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxi2po</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1cxgyej</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Hitting the beach</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxgyej</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1cxguws</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>aieyf + foxfire by mooncat 🧜‍♀️💎</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvhfw1ho2u1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1cxgjuu</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Boa Constrictor by Mooncat</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7pnu66fe0u1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1cxge34</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Need help to get to the next level.</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxge34</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1cxg2a4</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>I acknowledge the silliness of this question, but what makes some polishes "glow"?</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cxg2a4/i_acknowledge_the_silliness_of_this_question_but/</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1cxf5on</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>The "visible staining under clear nail envy" look I've been rocking the past week has gotten me as many compliments as my actual manis 😅</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cxf5on/the_visible_staining_under_clear_nail_envy_look/</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1cxcqcm</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>We have Flower Child at home</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxcqcm</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1cxcidf</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>I blame this on you guys</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8es98r7z6t1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1cxa9o3</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>🩵🦩Pink Flamingo🦩🩵</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxa9o3</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1cx9x90</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Lennnny! A new favorite</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nsruircdns1d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1cx8znw</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>PSA: Zoya promo</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cx8znw/psa_zoya_promo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1cx8zlq</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Lisa Frank nails on my gf!</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zpxswxs5gs1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1cx88e1</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Best baby pink polish?</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cx88e1/best_baby_pink_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1cx6ndx</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Cotton Candy - First time blooming gel</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cx6ndx</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1cx5pay</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>I was craving rainbow nails</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cx5pay</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1cx4x4t</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Tips for getting started with gel polish?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cx4x4t/tips_for_getting_started_with_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1cx3od8</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Electric sheep dupes?</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ev0876mmzq1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1cx3gfl</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Is this good nail growth for about a week? How do I go on about improving the look of the cuticles?</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cx3gfl/is_this_good_nail_growth_for_about_a_week_how_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1cwbc8b</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My mani for world bee day! </t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kpfwn5p8vj1d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1cxukyi</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>The set of impressionism</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxukyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1cxug79</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails product </t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://pronailcomplex24.com/text.php#aff=Luca11105</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1cxtad8</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>All my nails sets this year so far</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxtad8</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1cxs8j0</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Broken 🧚🏽‍♀️ glass? .... I don't know what to call these</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxs8j0</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1cxs2u5</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>fairycore nails🩷🧚🏻</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxs2u5</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1cxpohn</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>babyboomer acrylic nails</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5u1ghv53w1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1cxpnqb</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>3d nail art acrylics</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxpnqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1cxnuvc</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Just did this today. What you guys Think ? IG@NailsByTim6</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wad0m8ramv1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1cxmgil</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>🕸️🕸️🕸️</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxmgil</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1cxlf4t</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Plant Nails</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxlf4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1cxlavj</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>🐾🐈‍⬛❤️🐈🐾</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxlavj</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1cxjhvy</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Pink and flowers</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxjhvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1cxin5e</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Inspired by French landscape paintings, what do you think about this nail art set?</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r54oqs9ffu1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1cxhdsc</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Chappell Roan themed press ons</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxhdsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1cxh8fq</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Was feeling summer-y 🐸🍒🐻🍋</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o3qqoa8e5u1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1cxgdh4</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Champagne sparkles</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxgdh4</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1cxbpbh</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Creating some press ons ready for festival season </t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/smfg1z9w0t1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1cxaj9c</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Koi fish nails</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s7dvwg34ss1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1cx99pd</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Playing with magnets♡</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1c7fnczeis1d1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu May 23 08:08:58 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_26.xlsx
+++ b/data/2024_05_26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C612"/>
+  <dimension ref="A1:C776"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10838,6 +10838,2794 @@
         </is>
       </c>
     </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1cyn2x1</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Grad Nails 🙏🏻</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqobrprjp42d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1cxyrw3</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Would gel x, hybrid gel, or nothing be best for my brittle nails?</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9qmi3qp7zy1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1cxz3bf</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Advice on nail drill?</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxz3bf</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1cy4hsj</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Allergic reaction to gel?</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cy4hsj/allergic_reaction_to_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1cy7azr</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Ever since I developed a gel allergy I’ve had to learn to make do, and I’m honestly loving it!</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy7azr</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1cy7rnf</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Yogo zombie base vs dgel signature base, which one?</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cy7rnf/yogo_zombie_base_vs_dgel_signature_base_which_one/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1cy8mpk</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>These nails took forever, but love the outcome 😍</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy8mpk</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1cy9mfs</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Natural Nail Progress</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy9mfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1cy9myb</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Extensions? Fill? Gel vs gel x?</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cy9myb/extensions_fill_gel_vs_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1cyeacj</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Moss agate nails for my bday</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyeacj</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1cyfqt6</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Nail tech painted the glare from the inspo photo onto my toenail!</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyfqt6</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1cyhtfo</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>HELP! What method of manicures should I be getting for strong, healthy nails? This year I have 4 weddings plus pre-wedding events AND a baby shower. My natural nails grow long, strong, &amp; quickly but after my 3rd or 4th gel mani in a row, all my nails are weak, bendy, &amp; breaking. Press ons?</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyhtfo</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1cyijb5</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Attempted to soak off acrylic nails at home and this is the result. What should I do?</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyijb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1cyjdl2</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Tried the glamrdip kit for a home nail set</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0m8arsipj32d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1cyjpew</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>minimal men nails🌑</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyjpew</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1cyltq1</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>gel x on my sister</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ty0zn6u6a42d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1cylidr</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail health/healing </t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cylidr/nail_healthhealing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1cyl1c1</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>do i have to use tips for gel x?</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cyl1c1/do_i_have_to_use_tips_for_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1cykxmb</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>2.5 weeks in… builder gel is a game changer 💕</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uv3xkm21042d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1cykxk8</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t xml:space="preserve">question about monomer </t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cykxk8/question_about_monomer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1cykfh3</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Bunny nails ❤️</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4bpqn94ju32d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1cykddb</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>LA Girl Special Glaze Effect</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fjtjoskvt32d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1cyiu5a</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>I'm in love</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyiu5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1cyi05o</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/shmah1vd632d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1cyhsyv</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>What do you think of the color combination?</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9d8veauh432d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1cyhgoi</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Brand review?🇨🇦</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wssapu6c132d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1cyh69y</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Got these gel-x nails done the other day. Not sure what I expected but I don't know if I like them. What do you think?</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyh69y</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1cyh26m</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Love my nail girl🩷💙</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2wkjvhfox22d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1cygouf</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Girlfriend spent 3 hours and $200 and hates her nails — what should she do? </t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cygouf/girlfriend_spent_3_hours_and_200_and_hates_her/</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1cygmft</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Every set I’ve had in 2024 (so far)</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cygmft</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1cygjth</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>first time doing 3D nails 🍓</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cygjth</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1cyg7sq</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>French mail stamper</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cyg7sq/french_mail_stamper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1cyg01w</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>My first time doing flames</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0q5inppyn22d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1cyfzyh</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>My nail tech knows me so well</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyfzyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1cyfxhm</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are we into dark colors and muted colors or is it not a summer vibe? </t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyfxhm</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1cyfnm2</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Red❤️</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ewl8f5sk22d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1cyfk5t</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Never do matte but i kinda like these because of the mix of gloss in it</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyfk5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1cyffjn</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>One of my most beautiful designs 😍</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rw9bz6nsi22d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1cyf682</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Are these poorly done?</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyf682</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1cyf0mz</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>My first time getting an acrylic overlay.</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9jc41p6f22d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1cyegdr</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Gel X Set</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eilms5daa22d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1cyecps</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Black and white flower nails</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyecps</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1cye0hr</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>New set, do you think the design is original? Personally, I loved them 🦋</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8iqc9e3m622d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1cyc2oa</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>How can I heal my nail?</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qlc1sgclr12d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1cyc5o9</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Can I get French tips when I get these filled?</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v92f8748s12d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1cycixh</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Went to get a French manicure today at a salon I'd never been to</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cycixh</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1cyd8a5</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Am I valid to feel my nail salon did me wrong?</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6e0gfdgc022d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1cydu17</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>new set, opi press ons. i think i’m getting the hang of this!</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cydu17</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1cydsy2</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Love these!</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cydsy2</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1cydmcb</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are your favorite press on nails? </t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cydmcb/what_are_your_favorite_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1cyddb4</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Simple black frenchies 🖤</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a6zdjv0g122d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1cyd99q</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Help! Struggling with Dry Spots Around My Nails 😩</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u54pqahk022d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1cycsr2</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>My nails I did today 🥰</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cycsr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1cycs1v</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>My nail lady slayed it again !</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6elu6h7xw12d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1cybsyj</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Best nail length for beginners?</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cybsyj/best_nail_length_for_beginners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1cybsgz</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>My nails have never been healthier!</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cybsgz</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1cyb93n</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Wanted to do something different</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dhf3z0bgl12d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1cyavqd</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>hello kitty!</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdhwvzlqi12d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1cya8up</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My 15 year old sister started doing nails in January. Here are some sets she’s done for me! </t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cya8up</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1cya8d6</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>I want to buy my GF a kit she could take with her to the studio. What are some great, quality kits to consider?</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cya8d6/i_want_to_buy_my_gf_a_kit_she_could_take_with_her/</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1cy90m0</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Nail Charms</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fpq4qrjt412d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1cy8qpl</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Fruit nails 🍇🍒🥝</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy8qpl</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1cy7b7z</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>A website that allows you to upload photos and find nail polish colors closest to the ones in the image</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cy7b7z/a_website_that_allows_you_to_upload_photos_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1cy78sw</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How can I get better !? It’s been a year and I still am not great </t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy78sw</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1cy6bl8</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>$1.97 off SHEIN lol. But I love them despite the fact that I can’t do anything with them at all, except sit here and look cute.</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gbora8cjl02d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1cy53t3</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Nail lady forgot top coat on my acrylic nails</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cy53t3/nail_lady_forgot_top_coat_on_my_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1cy54i1</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Did my own nails and regret it</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kk48lbnxc02d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1cy5813</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t xml:space="preserve">National Goth Day nails ⛓️🖤 (inspo second pic) </t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy5813</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1cy68sh</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Hands of a goddess</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/15ukwblzk02d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1cy5xd6</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t xml:space="preserve">strayed away from usual almond nails </t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wpcb5wphi02d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1cy5usd</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>My fresh festival nails🖤</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy5usd</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1cy5gv1</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Vacation nails</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dw7ovocf02d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1cy5e8j</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Modelones soft gel tips - yay or nay?</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/awdyl2due02d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1cy54d3</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Help please!</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy54d3</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1cy5287</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Pastel colors 🩵💚🩷💜</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy5287</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1cy47hz</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alternatives to Acrylics for Nail biting? </t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cy47hz/alternatives_to_acrylics_for_nail_biting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1cy40zf</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail biting </t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cy40zf/nail_biting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1cy33ld</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>🖤</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy33ld</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1cy2war</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye nails!! </t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy2war</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1cy2soe</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>My nails this week</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bofd4ao2wz1d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1cy2k29</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>I'm in love</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy2k29</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1cy23pp</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Hair gel overlay &amp; nail are cracked</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1d2v42oyqz1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1cy1keu</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>birthday set!!! any other gemini’s getting dope nails for their birthday? 💕</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy1keu</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1cy1dm0</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Which Kind of Nails Work Best for the Beach?</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cy1dm0/which_kind_of_nails_work_best_for_the_beach/</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1cxzq8k</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>summery nails☺️🩵</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cz2ufwjy7z1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1cxzp1m</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>New Press Ons</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pxbjay0n7z1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1cxz8mr</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>new to nails</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxz8mr</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1cxy3tq</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel at home on my natural nails!! Super proud but the tips are so yellow!! anyone knows how to prevent that? </t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxy3tq</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1cxwoeq</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>This set is perfect for halloween</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2llwcs42cy1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1cxvvi7</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Purple galaxy nails 💜</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7eb5zqfh2y1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1cxv8bs</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>How long for SNS full removal and new set?</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhlr6puutx1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1cxv7dq</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>First Ombre 🥰</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxv7dq</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1cxv2f2</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Are these air pockets?</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxv2f2</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1cynba6</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Crystal Lake // Mood Ring</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cynba6</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1cyn02c</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This rocks! </t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3nbpqz9jo42d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1cyjq5z</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>haven’t done any nail art in a while and found this in my camera roll</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wd4abwvan32d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1cyjc78</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Tips for a beginner?</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cyjc78/tips_for_a_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1cyjbr0</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Caught my nails looking good in the parking lot</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n28c1a47j32d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1cyi5gh</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails keep distracting me... like, excuse me, I'm trying to rewatch Fringe! </t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v8xn5s8t732d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1cyh241</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Omg, Help!!</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyh241</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1cyghzy</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Anyone else feel naked with a solid cream mani!?</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvqjfezgs22d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1cyghve</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Nail polishes that match these eyes?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjipl5lfs22d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1cygfne</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Twinkled T Cutting Stock/Major Sale</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cygfne</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1cygc6r</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>🤯 welp… guess I need more magnets now</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vksms5f1r22d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1cyg74c</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t xml:space="preserve">French nail stamper </t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cyg74c/french_nail_stamper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1cyg2dt</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>I was influenced</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvd5ygbko22d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1cyf4eq</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Rose Jelly - Cirque Colors</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyf4eq</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1cyeuvw</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>moody bluesin’ 🩵🕊️💙🌊🩶</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/086wdxtqd22d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1cyddsl</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Simple black frenchies 🖤</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bobwsq0k122d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1cydaom</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Magnetic Swatch board</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cydaom</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1cycty9</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>How do you pick toppers?</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cycty9/how_do_you_pick_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1cycroj</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>I love these! Nude base, purple chrome powder, with gold 🌛🌛 and ⭐️⭐️</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bf7osz8uw12d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1cyclud</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Still on the hunt for a good nude. How does this one look?</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kdxcx75nv12d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1cyc4ub</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Mooncat Mercury's Tears</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyc4ub</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1cybalb</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>For anyone else who was disappointed that Treachery in the Blue was less pink and more beige than the pictures, I think I found a solution! (+ Cat Tax)</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cybalb</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1cyaz97</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Looking for a dark grass/forest green dupe like these (pics)</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cyaz97/looking_for_a_dark_grassforest_green_dupe_like/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1cya1de</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>bright colors for summer!</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ufb4baa8c12d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1cy9pns</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>My first two attempts at press on painting!</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pggon62z912d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1cy8fbz</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Let’s say HYPOTHETICALLY you are painting your nails and on finger #8 you realize….</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cy8fbz/lets_say_hypothetically_you_are_painting_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1cy8ck3</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I found this old Essence nail polish and I remembered how nice it is </t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0pyf41yz02d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1cy87fy</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>ILNP - Celeste</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy87fy</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1cy849v</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Mooncat lady, I know you’ll read this:</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cy849v/mooncat_lady_i_know_youll_read_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1cy7mxf</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Baby’s first Mooncat 🌷💕✨</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/pVhOcEV.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1cy7m63</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat Prickly Pear </t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2w2d4d6su02d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1cy7kjz</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Midnight Thunderstorms </t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z7oafokgu02d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1cy74ld</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Mooncat's 'Shattered Glass' making me feel better about my crusty hands 💜</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy74ld</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1cy6tlb</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Each little slug here cutting a rug </t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53ciayw6p02d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1cy6gbo</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Some recent favourites</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy6gbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1cy69rc</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>My son decided I was going to do his nails last night as well as my own. He chose polish colors for both of us!</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy69rc</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1cy65k3</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Am I Everything You Fear? ✨️😈</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy65k3</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1cy5wsg</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Glowy Light Dragon!</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy5wsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1cy5q6i</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>My nails feel look like they are glowing 😍</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy5q6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1cy5ktm</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Which shape looks better?</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy5ktm</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1cy5hls</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Favorite brands for duo/multi chromes with NO holo glitters?</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cy5hls/favorite_brands_for_duomulti_chromes_with_no_holo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1cy5eho</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Manicure/Pedicure</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cy5eho/manicurepedicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1cy4cyd</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>flower child as a topper 🌸🦋</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy4cyd</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1cy44gm</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>🌈Nyan Cat🌈</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy44gm</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1cy3hjx</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Sabertooth</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy3hjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1cy1m22</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>My roommate called them “Rituals Japanese spring collection” 🌸✨</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy1m22</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1cy135t</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>A few recent Prism Polish UK manis</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy135t</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1cy10z4</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Hi! I’m new here and on the hunt for a shrink free top coat</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lry3firkiz1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1cy0uza</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>To All Who Ghosted Me</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x66pvsqbhz1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1cy0l2o</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>High Roller 💜😈</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/535gfxz4fz1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1cy05dt</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Newbie questions - Acrylic</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy05dt</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1cy04qv</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>How do I prevent this lifting?</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy04qv</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1cxzi7m</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Talk to me about quick dry top coats? </t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cxzi7m/talk_to_me_about_quick_dry_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1cxyfoe</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Cirque Vice Comparison Swatches</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxyfoe</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1cxxjql</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Have you tried thermal polish?</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cxxjql</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1cyn56i</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>The long-awaited forest-themed nail art has finally arrived! 🌿✨ Today, I’m excited to share some uniquely styled forest-themed nail designs with you all!</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyn56i</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1cyjoro</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Deleted the other post to add the finished product :)</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/853hpowvm32d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1cyj6xd</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>how do nail techs do this type of art?</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oofgsdqth32d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1cyj3yu</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>my nails</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/twa64p50h32d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1cyhu5n</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>I need help choosing my next nail design! Do you have ideas? I currently have these, what do you think?</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6y1rhw3t432d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1cyhsqt</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>What do you think of the color combination?</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ambdrzrf432d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1cyf8t5</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Nails with cherry. what do you think?</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5pkhc66h22d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1cy9lor</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Pop art nails! 🥰 My very first homemade press ons</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9eq1lcf5912d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1cy8ack</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Builder gel with transfer foils</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5phaorkz02d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1cy897j</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Gel almond micro frenchied</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/084swuucz02d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1cy7z84</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vokmqrtbx02d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1cy71hn</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Nail art ideas?</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy71hn</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1cy5927</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Nails red 🖤</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8irs9nud02d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1cy384b</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Some of my fav I did this month!</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy384b</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1cy1jii</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Spring/summer rainbow ombré!</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cy1jii</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1cxyfs3</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Bridgerton inspired</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k92rc9z0wy1d1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri May 24 08:08:53 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_26.xlsx
+++ b/data/2024_05_26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C776"/>
+  <dimension ref="A1:C947"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13626,6 +13626,2913 @@
         </is>
       </c>
     </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1cz8xbu</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Nail damage from e-file</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxr64pypy92d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1czea7x</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Short or long nails more appealing?</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/btk6v0i5jb2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1cyocif</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Nails + Nail Bed Progress (3 months)</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1a1r6ww552d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1cz0ro5</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>I feel like stickers would be the ultimate hack if they didn’t tear so easily</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz0ro5</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1cz55sm</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t xml:space="preserve">can someone plz explain: solar vs UV vs biogel? </t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cz55sm/can_someone_plz_explain_solar_vs_uv_vs_biogel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1cz5qtb</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>DIY dip: No UV light needed?</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/atxdzxnp692d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1cz7aql</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Pointer finger nails splitting under acrylic</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cz7aql/pointer_finger_nails_splitting_under_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1cz8w69</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Is it a trend to keep your toe nails long?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cz8w69/is_it_a_trend_to_keep_your_toe_nails_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1czaxu2</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>end of an era</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmc9qk68ia2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1czcdel</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Y’all I kicked the habit! and have more confidence in my Gel X ability</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czcdel</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1czct5u</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>I just got my nails done for the first time and I want the OFF!!</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1czct5u/i_just_got_my_nails_done_for_the_first_time_and_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1cze0n4</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>I wanted to feel like a princess✨️ She nailed it.</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upqdsr3wfb2d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1czdzqj</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tips to stop gel nails chipping/ UK product recommendations </t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1czdzqj/tips_to_stop_gel_nails_chipping_uk_product/</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1czds0p</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Me taking a picture of my nails 4 weeks later🌝</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwt9k9c2db2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1czd4qx</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>My nail tech has moved to another city. I had to go to a new tech</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p15lbvvi5b2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1czd179</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Filed and buffed</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czd179</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1czd0jc</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Filed and buffed </t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1czd0jc/filed_and_buffed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1czchr9</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My second time using rhinestones/embellishments. I love these! </t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czchr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1czcb5e</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Iridescent set</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/obbalbzcwa2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1czcavc</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Very overdue manicure</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czcavc</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1czc3l0</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>I need help</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czc3l0</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1czc3kn</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Haven’t done my nails in a while. Missed my red bottom claws </t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czc3kn</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1czbl6b</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>My nail tech is so 💕💕💕</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mzyddqgwoa2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1czbbps</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Going to get my nails done!</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1czbbps/going_to_get_my_nails_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1czb8ah</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>✨sparkles✨</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czb8ah</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1czb2jr</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>“Jelly” nails for petite nail beds?</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czb2jr</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1czb29v</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Gem vibes</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1de00obgja2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1czar2v</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>In love with my new set! 😍</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9cxygmdga2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1czao2n</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some nail wraps I've over the last 6 months. </t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czao2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1czab7p</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>First time growing out my nails...</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1czab7p/first_time_growing_out_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1cz9h9d</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Went with a mermaid chrome to kick off the summer months. </t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76dkean24a2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1cz8wff</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Ocean Nails 🌊</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6ynrv6jy92d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1cz8jbq</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>My husband called them $1000 nails</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz8jbq</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1cz7n65</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Pretty proud of these clouds</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ruknhtmxm92d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1cz6w8g</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0cj9bdgg92d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1cz6fax</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Blue Eyes 👀</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/te0zzg8fc92d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1cz68qv</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Can I get a French tip with short nails?</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4hdblziwa92d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1cz663n</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>a couple days ago, i wanted to get my nails done.. soo.. 🙈</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ftsg554aa92d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1cz64pn</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is the easiest + long-lasting method for doing long nails at home? </t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cz64pn/what_is_the_easiest_longlasting_method_for_doing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1cz5b9m</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Gel Polish for a newbie</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cz5b9m/gel_polish_for_a_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1cz4qt7</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>can i remove these without a drill?</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cz4qt7/can_i_remove_these_without_a_drill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1cz4glo</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Neon cat eye shorties!</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz4glo</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1cz4f98</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>My nails match my pepper spray.</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zvg7ie8bw82d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1cz46oe</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cz46oe/is_this_normal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1cz41nv</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Did my nails</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz41nv</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1cz3si8</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Weird new gel polishing technique?</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cz3si8/weird_new_gel_polishing_technique/</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1cz3q0u</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>💙 ILNP Bluebell 🧡</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz3q0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1cz3il4</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Did my nails today for the first time in a while</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz3il4</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1cz2qz9</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>My girlfriend made my nails, any feedback for her on what she could do better ?</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz2qz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1cz2lr2</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>They took me a while but I absolutely love them 💅</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz2lr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1cz2ijx</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Apres v. Acrylics</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cz2ijx/apres_v_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1cz2i9s</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Could anyone possibly suggest some nail tech names please for my daughter 🙏🏼 </t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cz2i9s/could_anyone_possibly_suggest_some_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1cz29f5</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>First time with red nails..</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz29f5</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1cz25qw</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>This set gives me Daphne from Scooby Doo vibes 🌺</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t8vacrvcf82d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1cz1oij</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Two at once 😔</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdkrbevtb82d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1cz18dc</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Just got the cutest ombré nails ever</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0tawtk1j882d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1cz0oxa</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>recent press on nails i’ve done :,)</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2dzun7l482d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1cz0e1y</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Love the nails I did today</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cjrtlcnb282d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1cyvt08</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>This always happens to me</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v8vnl0ij472d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1cywxmh</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>How do I get more slender nails after this? Do I have to start over?</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cywxmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1cyx1my</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can gardening &amp; decent nails coexist? </t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyx1my</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1cyya3w</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Inspiration and results…nailed it.</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyya3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1cyzlph</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Botanical porcelain 💙🤍</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyzlph</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1cyzo8n</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>First gel set of the season!</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyzo8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1cyyst0</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first try doing dip/gel nails! </t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyyst0</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1cyysj3</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>My 74 year old neighbor asked me to paint her nails… I asked her what color she said “I want THAT color!!” Now we match lol :)</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3shu86hiq72d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1cyyiu6</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>My dollar general nails</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rsqg22cho72d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1cyyeex</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Simpler design I just did, but it’s so cute</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6q07x7kn72d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1cyy5t7</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>“Leave Him On Red” ❤️</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyy5t7</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1cyy3wg</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Before and after </t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyy3wg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1cyxwmj</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>base of the french tips too pink</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxr0j02wj72d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1cyxuqo</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Help! Advice for bitten nails for Prom (UK)</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cyxuqo/help_advice_for_bitten_nails_for_prom_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1cyxl5j</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Light Pink with Mixed Metal Foil Accent Nail</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyxl5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1cyxe5e</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Was going for goth vibes, I think she did that perfectly 🖤❤️</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyxe5e</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1cyx37x</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>gel nail strips</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyx37x</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1cyx0fc</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Prom nails</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/plgq4qabd72d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1cywwuu</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Nailed It</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bu2vxf4kc72d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1cywb0c</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Second GelX Attempt!</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cywb0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1cyvtul</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>New fill in and I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyvtul</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1cyvt9n</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Sweet lace nails!</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cpb4bs2l472d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1cyvqqe</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Just wanted to share my birthday nails</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/spva0nh2472d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1cyvany</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>My nails were in really bad shape so I started putting on and painting press ons until they get a little better</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyvany</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1cyvanm</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>🖤</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lq98pe7q072d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1cyv59z</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Anyone have any good LA based nail tech recs? Thank you in advance! 💅🏼</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cyv59z/anyone_have_any_good_la_based_nail_tech_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1cytpam</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Second attempt at the mess they made on my nails a few days ago.</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v56hpl7no62d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1cytnd2</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Nails🥺</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cytnd2</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1cytdo7</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t xml:space="preserve">"Butterflies are born 2x but die only 1x 😌" -Me&amp;my high thoughts one day </t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/05k1i4s7m62d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1cysykn</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>First set since November!!</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cysykn</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1cyslkn</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Cirque for the Spring Win!</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hm810r8of62d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1cyrj9h</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>really proud of these pressons i made!!</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyrj9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1cyrezj</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Todays clients first time ever getting her nails done. She was superhappy! </t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mynbz22562d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1cyqk2s</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Aprés over Acrylics?</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyqk2s</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1cyqf9i</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Looking like waves</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyqf9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1cyq4zx</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>At this point I let my nail tech do what she wants. She kills it.</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vvh9eqjwr52d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1cynwnq</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Eclipse 🌑</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dfu5spi9052d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1czefpn</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Hamster nails I just did :)</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czefpn</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1czecuv</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>What shape are these?</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czecuv</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1czcopf</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>My Experiment: cuticle oil and slowly pushing the proximal nail fold back</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czcopf</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1czcfb2</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Newb starting out: recommendations for starter must-have products?</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1czcfb2/newb_starting_out_recommendations_for_starter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1czc6n3</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Nails spontaneously falling of in crescent shape??!</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1czc6n3/nails_spontaneously_falling_of_in_crescent_shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1czc6hj</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Nails spontaneously falling of in crescent shape??!</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1czc6hj/nails_spontaneously_falling_of_in_crescent_shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1cz94xd</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>New favorite neutral!</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz94xd</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1cz4k3i</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Happy dance!! Nothing is broken 🥹 (proof!)</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz4k3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1cywuva</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dollar Tree polish for the win!🏆 </t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cywuva</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1cz1j5o</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>How should I organize my swatch wall?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pxa6g9lqa82d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1cza3md</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Simple ombre dip</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/spcgrcb5aa2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1cz9zk8</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>How often do you buy polishes? And how often do you re-wear polish?</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cz9zk8/how_often_do_you_buy_polishes_and_how_often_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1cz9yt1</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Mooncat Dragon Scales - so shifty</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz9yt1</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1cz9saw</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>ILNP Chai Latte ☕️</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz9saw</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1cz9jpd</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Full Scream Ahead</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz9jpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1cz90yf</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>MC Dark Horse vs ILNP Abundance</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz90yf</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1cz8wxa</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Schools out for summer!</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz8wxa</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1cz8wdy</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Are all glitter smoothing topcoats the same?</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cz8wdy/are_all_glitter_smoothing_topcoats_the_same/</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1cz8uaa</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Yellow Smelt Quartz</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz8uaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1cz8jat</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Houston, we have velvet</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz8jat</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1cz7wkz</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Should I move to a new nail tech? (greenies, lift, etc.) Bonus question, shoud I removed my nails?</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cz7wkz/should_i_move_to_a_new_nail_tech_greenies_lift/</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1cz7fps</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>You Will Be My Undoing</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz7fps</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1cz7f3i</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink glaze 💖 </t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ema64ayk92d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1cz77gj</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Doing my nails makes me wish we had another thumb on the other side </t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cz77gj/doing_my_nails_makes_me_wish_we_had_another_thumb/</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1cz72fe</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Fairy Dust as a topper &gt;&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz72fe</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1cz5wvc</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Kitty Approved 🐈‍⬛️</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz5wvc</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1cz5nca</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Should Have Been a Shenanigans</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz5nca</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1cz4dci</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Freshly bitten 🩸</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz4dci</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1cz440b</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Isle of Capri SOL?</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz440b</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1cz3pc8</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>💙 ILNP Bluebell 🧡</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz3pc8</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1cz3i0z</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Anyone familiar with Nuvail?</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cz3i0z/anyone_familiar_with_nuvail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1cz3gv6</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>“Sunken Splendor”</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz3gv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1cz3gb6</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Day 6 mani with ORLY morning dew</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/to058xc0p82d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1cz3bl9</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Uh oh</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jg8cuc8zn82d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1cz39ta</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Pink Polish Recs</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cz39ta/pink_polish_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1cz33h7</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Why does my nail polish always chip/smudge in this exact spot?</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/civ7ucl8m82d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1cz32ld</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Distracted on my walk</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxkjiet2m82d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1cz1z2e</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Dupe for Covergirl Glosstini in Rogue Red?</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cz1z2e/dupe_for_covergirl_glosstini_in_rogue_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1cz1kt4</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>The people have spoken</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz1kt4</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1cz0ig4</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>ILNP velvet skittle mani inspired by another laqueristas post</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cz0ig4</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1cz0hpc</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Fairy Dust at 10k feet elevation! ✨ ✨</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6pmqfl83382d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1cyzlr7</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>First polish from Mooncat sale… you already know</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyzlr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1cyzjs8</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>I need more fingers 😭</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3lcrf2l3w72d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1cyzgud</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This one is indeed the devil </t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9njxg0jv72d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1cyz77i</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Back with another red…Hot Chicken!</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bsrnyhnkt72d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1cyykd1</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>ILNP New Day and ILNP Horizon on accent finger</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e4hri7hso72d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1cyyjdo</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Tbt milk bath nails</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ezphpqhlo72d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1cyy4i7</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Playgirl 'Russia'</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/OrcUQgG</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1cyxb2w</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Love me some squiggly lines</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vlg2750kf72d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1cyum2e</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do I have corpse nails? </t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pb179ydmv62d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1cyucxv</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Anyone have experience with Glam Polish customer service?</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cyucxv/anyone_have_experience_with_glam_polish_customer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1cyu6bj</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>I don’t do my nails for men. I do them for the teenaged baristas at my local Starbucks.</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xoi0nwkas62d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1cytmtz</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Sugar Fix</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgxnn2h4o62d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1cyrzw1</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>So popular even kittens love her, ILNP Fairy Dust 💜🩷✨</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyrzw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1cyrswv</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>LynB Designs - Aquarius (The Water Bearer)</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gd54s0dn862d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1cyrgim</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t xml:space="preserve">To All Who Ghosted Me </t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyrgim</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1cyqthc</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>I love these color shifts with different lighting!</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u0ompwr8z52d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1cyntjr</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Eclipse 🌑</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ab7hqxp6z42d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1cynn2k</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Loving getting back into normal polish after years of gel!</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1k1wz6tw42d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1cze51y</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>🌈🌈🌈 (please forgive my sad cuticles 😭)</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2cvdrooehb2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1cz8t5v</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Vacation Nails!</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z192w5knx92d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1cz7v7o</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Butterfly wings</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9c2ua3k0p92d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1cz6fvr</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>i ❤️ my nail tech</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8d2mb9hkc92d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1cz2y93</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Nails for my 22nd bday</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4unk1r6l82d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1cyzm7b</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>3D my new style of design. What your? IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ypgmkflw72d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1cyz133</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Metanail Complex - Presentation</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://metanailcomplex.com?shield=577752ebueq7y63dtrgxxgqi41</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1cyy8tn</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Finally some sunny weather!</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyy8tn</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1cywd4x</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Que tal?</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qharggio872d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1cyvrap</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Pt. 2</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyvrap</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1cyvn5a</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Fun stuff lately Pt. 1</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyvn5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1cysoac</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>The galaxy on the nails. what do you think?</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t09j5kzag62d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1cys4t1</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>What do you think? They like?</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/diq7matqb62d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1cys2k4</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Les gusta?</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j6q13ef5b62d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1cyrqrx</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First go at tip extensions, dip &amp; cateye polish </t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8vq21no6862d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1cyqtsy</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lover girl set </t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h82yh1scz52d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1cyp7wz</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Some IceCream Nails I Made(gotta fix the cone)</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cyp7wz</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat May 25 08:07:45 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_26.xlsx
+++ b/data/2024_05_26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C947"/>
+  <dimension ref="A1:C1106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16533,6 +16533,2709 @@
         </is>
       </c>
     </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1d06gnc</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Need help learning gel at home !</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xbb1s31uwi2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1d0670f</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Ideas 💡</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uwclukqiti2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1d05doo</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Fancy fangs</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9o95spoji2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1d057ft</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Shot through the hearts 🤍🤍</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4101vg3ohi2d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1d04dg9</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Feeling absolutely FABULOUS today!!!</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/757v5fjy7i2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1d043ye</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>I couldn’t decide so my nail tech did… 🌈✨🌸💅</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d043ye</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1d03zem</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GelX Advice </t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d03zem/gelx_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1d03yov</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails that can be easily removed and put back on throughout the week? </t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d03yov/nails_that_can_be_easily_removed_and_put_back_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1d03g8f</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>In love with my graduation set</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k61opfltxh2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1d035n6</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Pretty sure this is now my favourite set I’ve ever had 🥰✨</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d035n6</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1d0334j</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Old post but I miss this pedi/heels combo😔😮‍💨 So appealing 🥰💅🏻</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9v4p8kjsth2d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1d02km5</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Where to find similar polish colours in Canada?</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d02km5</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1d027fe</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Would it be harder to scratch with gel extensions?</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d027fe/would_it_be_harder_to_scratch_with_gel_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1d025jt</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Perfect funny bunny SNS</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sz7h9l37kh2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1d01h7z</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Opinions</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d01h7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1d015rh</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Love this set</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ubace59ah2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1d00k9t</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Apres Memorial Day Sale (Gel X)</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d00k9t/apres_memorial_day_sale_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1d00743</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Name that shape!!</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d00743</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1d002do</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Since moving to tokyo, i started using press on nails! The options here are amazing 🥹</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d002do</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1czzudr</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>can never go wrong with pink 🎀</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mb1shb3jxg2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1czzqxf</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Practice practice practice</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czzqxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1czzp2v</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>some jujutsu kaisen nails i did !</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czzp2v</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1czzatm</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Well. I tried.</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czzatm</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1czz2dw</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Doing gel x to my self tomorrow! Any new tips? </t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czz2dw</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1czz0wg</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Bears in space 🪐</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hbflcph3qg2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1czyeln</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Green mani</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bnuylmbukg2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1czybv4</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Neon 😎</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ftztb487kg2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1czxwiq</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Vacation nails for my friend</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5r7iv88lgg2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1czxbyp</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>WDYT?</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zk7j19hvbg2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1czx87y</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Very simple nails but I love the colour </t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zip2qwmzag2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1czx5j4</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>A little bit of green 🐞</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0y6cutmdag2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1czwkl4</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Monthly nails!</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gc3311pn5g2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1czvukn</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Daughter's Grad Set! </t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ate61qkxzf2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1czvsfb</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>I (31m) want to learn to do my wife’s (24f) nails, could use some help on where to learn/what to buy</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1czvsfb/i_31m_want_to_learn_to_do_my_wifes_24f_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1czvp9b</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>this year’s pride nails &lt;3</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czvp9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1czv0ys</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Made my first set of custom press ons! 🍓</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqm5gosftf2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1czuw0i</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>im obsessed i got my first russian manicure</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mc28xq4bsf2d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1czurup</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Obsessed 💖</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4nluphmerf2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1czuixt</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Paid $60 for this! 😭😭😭 how bad is it?</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2c2sfohgpf2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1czugnl</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Not used to short nails, but I'll be gardening this weekend and don't want to break them 🌸🌼</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czugnl</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1czuggp</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>My nails are summer ready I love my nail tech🍓❤️☀️!</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sst0vffwof2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1czu95q</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>An old set, I loved this shape 💜</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cwx8mq9anf2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1czt8tz</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Just did my nails do you like ‘em?</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czt8tz</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1czsygo</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Butterfly Wings 🦋</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czsygo</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1czsu37</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>tips on thinning sally hansen miracle nail thickener</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1czsu37/tips_on_thinning_sally_hansen_miracle_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1czskvo</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>The new nails, all natural length!</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7echyyjaf2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1czsape</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Burned by nail light?</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1czsape/burned_by_nail_light/</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1czsaim</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>I'm no pro, but I tried to do sapphire velvet nails using cat eye polish</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ke7hpiyo7f2d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1czrpow</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>French nails with Natural tan base 💅</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjlutbyy3f2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1czr0vl</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>painted some press-ons</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czr0vl</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1czqxbj</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>TJ Maxx nails &gt; Salon</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czqxbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1czqvej</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Dark Chocolate</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5w71qhlxe2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1czqtz5</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Chrome nails, yay or nay? (PICS)</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqkjbdeaxe2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1czqfzw</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New pink French tips 😍 I am OBSESSED </t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pk325kzaue2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1czqaiw</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>32 days growth</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czqaiw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1czq4sl</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Maybe you can tell me I’m just being dramatic?</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czq4sl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1czpq5l</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed 😍 </t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fezp4duvoe2d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1czpq4r</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My friend's nails I did </t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czpq4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1czpi7f</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Messed up on my first set of press ons 😆</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6nynz6ane2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1czp0i9</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Baby pink frenchies by me</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czp0i9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1czosif</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Summer Nails 💅</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czosif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1czoneg</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Could someone please explain why you can't paint black nails on elderly?</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/idwkn9msge2d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1czod6o</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>One of the last nails I did for my grandmother, she always told me that the red reminded when she was young</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czod6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1czn1qy</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Look, Ma. I’m a 🦄</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1q1s96lg4e2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1czm5og</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried a different color, I usually stick to red and nudes. </t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2s6a4b5ixd2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1czm0q4</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Thinking back on an old manicure while waiting on my next appointment!</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pqb9ctlgwd2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1czlsej</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💅🏻 in love with this design </t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yd3o1mlnud2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1czlp2n</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Simple and quick milky flower nails. Not my best but baby approved.</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0cdqfyfxtd2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1czlhit</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Made new pink ombre press on nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czlhit</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1czjds7</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>My Mooncat order arrived! ✨️</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czjds7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1cziiy3</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Nail shape help!</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n7algdy11d2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1czie3e</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Butterfly wings guess how long these took</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eg5ux80lzc2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1czgxmt</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>First time doing a stiletto-y shape and I am so delighted</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vz8go510ic2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1czgpq8</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>The process of making my bday nails!</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czgpq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1czgli2</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Was $65 too much??</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czgli2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1czggvz</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>XL Stiletto Gel-X Pink Sparkles</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czggvz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1czg530</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Extra wide press ons?</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1czg530/extra_wide_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1czfy6y</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Matte red ❤️</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czfy6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1d073cr</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Cirque Polish Plastik comparison (2017 vs 2024)</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d073cr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1d05x0p</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Dazzle Dry - Coastal Cabana swatch</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d05x0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1d052sm</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>is it worth painting my nails if I work in a kitchen?</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d052sm/is_it_worth_painting_my_nails_if_i_work_in_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1czxnki</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>How are you guys dealing with shipping costs?</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1czxnki/how_are_you_guys_dealing_with_shipping_costs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1czxc2d</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Green nails with gold stamping (the green is lighter and more sparkly irl, but I couldn't capture it)</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1fla3mivbg2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1czuxw3</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Large-sized adhesive tabs</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1czuxw3/largesized_adhesive_tabs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1d04seu</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wtf is this???? </t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lpgo1c4pci2d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1d0495f</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sparkly pond water </t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0495f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1d03nsm</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>HOHs shiny sister</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jdgilqvwzh2d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1d02tnk</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Perfect Trifecta </t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d02tnk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1d027n0</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Has Mooncat been reimbursing people for their polishes that arrive broken? Folks who had a broken one, what has your experience been so far?</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d027n0/has_mooncat_been_reimbursing_people_for_their/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1d01wyq</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Cirque Jelly nail polish — the love of my life</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d01wyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1d01j13</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Iso pastel comparison</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d01j13</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1d00zxt</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Getting a weekend away for my tenth anniversary. It was a toss up between bringing all my supplies and enjoying kid-free manis, or getting something elegant and longer lasting. Went for something in the middle. Two questions in comments.</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d00zxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1d00j1t</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>How long do I have to grow my nails and how I do cut them to my desired shape (almond)?</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d00j1t/how_long_do_i_have_to_grow_my_nails_and_how_i_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1d00dvm</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>There's no way it'll happen to me... 🙃</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d00dvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1czzr9d</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>My first ILNP and my first “regular” manicure in years!</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hwyyf46qwg2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1czzocb</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>first try brand: nails inc</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/thxcswzyvg2d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1czzlmi</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Just got my first Lurid order in and oh my GOODNESS I’m in love</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/elfp3hd9vg2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1czzddu</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>MC manis &amp; broken bottles againnnnn</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czzddu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1czyszs</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>“Fig” jelly by Le Manoir #nofilter 😛</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k711q5w3og2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1czyoj5</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Took Mooncat's Millennia out for a walk and fell on love</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ivl5m6c6ng2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1czxrl8</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Space Fairy Nails! 🦋🛸</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gnnuv8lhfg2d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1czx9bh</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Mlem</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8o9laz18bg2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1czvsux</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t xml:space="preserve">do you put a top coat on swatch sticks? </t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1czvsux/do_you_put_a_top_coat_on_swatch_sticks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1czvprg</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Essie cactus &amp; orchid jelly</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czvprg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1czvm2b</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Can’t stop staring at my nails 😍</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofughtn0yf2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1czunvf</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Chipped Bottle from Mooncat</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czunvf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1czuc8c</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Dragon Scales</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czuc8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1cztk3j</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Sparkling Water 💦 for broken nails</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32qdck92if2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1czt9va</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Honey in a copper pot</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/WGSW0KE</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1czsfg0</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Am I too late for the Butterfly Trend? Instagram @charli.bell.9</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czsfg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1czs933</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Top coat?</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1czs933/top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1czs2mu</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>All of your polishes are taken away and you can only keep one to wear for the rest of your life...</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1czs2mu/all_of_your_polishes_are_taken_away_and_you_can/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1czrws0</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>New polishes! Help me pick my new mani</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czrws0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1czr6k5</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Finally got my hands on Lurid Lacquer Indomitable 💜</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czr6k5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1czr2ih</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>i painted some press-ons!</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czr2ih</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1czkolg</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Peeling/ popping off gels and acrylics</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1czkolg/peeling_popping_off_gels_and_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1czqy77</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Did I just put nail polish all over my fingers (Cuccio moisture replenish)</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czqy77</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1czquoh</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>The weather in oregon feels like fall, so I did a fall/tigers eye inspired mani</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czquoh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1czqslg</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Please help. What’s going on with my nails? (3 photos of my fingernails) </t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czqslg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1czq14h</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Mermaid vibes with Blue Lagoon🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czq14h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1czq0j8</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Why oh why did she have to be limited edition?</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2wf8csv1re2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1czpvha</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>This polish is SO glowy and beautiful, but it is also worth noting the undertones of yellow/orange pigment when looking at a non-glowing angle.</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czpvha</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1czpqxi</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>The Sky Above</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4tm47vq1pe2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1czpeig</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>So I spent some time perusing the Mooncat Facebook page …</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1czpeig/so_i_spent_some_time_perusing_the_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1czoxmr</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>This is my summer of neon pink and sparkles</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxb0twuxie2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1czosdl</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>What is the best strengthening base coat?</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1czosdl/what_is_the_best_strengthening_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1czo2o8</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>While you were sleeping, I studied the chrome</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czo2o8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1czo0sw</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Fruit set for a fruity girl</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czo0sw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1cznsai</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Most dangerous chores?</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cznsai/most_dangerous_chores/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1cznlgd</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Slight VNL in 2 coats?</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cznlgd/slight_vnl_in_2_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1cznkzc</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Lumen Glass Stars, holy moly!</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/02biw9sl8e2d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1czn2js</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Boobies In The Wild</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czn2js</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1czmxge</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>🤍🍊💙Cobalt &amp; Oranges💙🍊🤍</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czmxge</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1czm20t</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Jellies from Cirque/ILNP?</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1czm20t/jellies_from_cirqueilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1czlwtb</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Devil's Ivy fresh app vs 1 week later </t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czlwtb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1czlko2</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Be honest, is my holiday weekend mani not bright enough? /s</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czlko2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1czliag</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Mooncat and peeling/chipping?</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1czliag/mooncat_and_peelingchipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1czkuh7</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Hello Kitty nail stickers!🩷💕💖🩷</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czkuh7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1czkmhu</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>My first French!</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czkmhu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1czk3tp</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recommend solid builder gel brands? </t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1czk3tp/recommend_solid_builder_gel_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1czj6wy</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>She's here!!! ✨️</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czj6wy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1cziqfb</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Still obsessed with this shade! </t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqo0do493d2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1czijl0</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Heart of the Warrior inspired layering experiment 💖</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czijl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1czg0yy</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Tips on shaping your nails?</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1czg0yy/tips_on_shaping_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1czfqoi</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>ILNP Flower Child</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4yru9try1c2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1d06seo</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The new summer trend press on set </t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f0kwvzqi0j2d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1d067ok</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Every girl can shine.</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ciwv3ikrti2d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1d03atg</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>My boyfriend said this is the coolest manicure that I have ever worn.</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d03atg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1czzw0b</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>First time trying chrome effect</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvb3iegxxg2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1czziqw</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>This week's art - wiggles</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czziqw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1czx3g7</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>I want to show you the nails I did</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czx3g7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1czufue</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>My girl @nailedtothecounter went full chaos today and I’m here for it.</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rp6urskpof2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1czss1j</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Summer nails to match my noodles 🍜</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ik1glyz1cf2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1czsesu</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Am I too late for the Butterfly Trend? Instagram @charli.bell.9</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czsesu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1cznvfa</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Summer is coming ✨</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cznvfa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1czmnvl</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Acrylic full set with all hand-painted 3D art!</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psof7z7i1e2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1czlguy</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Working on being okay with not being great yet bc ( I have been doing this for so long ) I have not been doing this that long in reality lol</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1czlguy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1czl13h</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>The new summer trend. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/956gf4nmod2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1czgmsn</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>i ❤️ my nail tech</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/77lh6cz0ec2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun May 26 08:07:41 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_26.xlsx
+++ b/data/2024_05_26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1106"/>
+  <dimension ref="A1:C1269"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19236,6 +19236,2777 @@
         </is>
       </c>
     </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1d0w7s4</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>feelin’ sad. gave myself some miffy nails to cheer up a bit 🐰</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0w7s4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1d0vu7k</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Broken nail</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d0vu7k/broken_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1d0v4ci</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>White croc shorties🐊🤍</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0v4ci</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1d0urzm</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>What should I do next?</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0urzm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1d0u5lg</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Nude/pink color recommendations</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rk0aucs2fp2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1d0tu68</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Surprise nails</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4g3lh5fbp2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1d0sfen</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>new nails y’all!! what’re we thinking?</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0sfen</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1d0qvpf</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Couldn’t Stop Staring </t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0bjea5weo2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1d0s1vu</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>I tried my hand at gel nails and they're a little. . .messy. I would also like advice on my nail shape, please. Square? Almond? Round?</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0s1vu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1d0ru72</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>OBSESSED!!!!</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0ru72</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1d0ricj</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>OPI’s Do You Sea What I Sea?</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0ricj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1d0rgar</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>French Tips</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7g0cz0kyko2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1d0rfjw</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Oxblood red/vampy colors?</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d0rfjw/oxblood_redvampy_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1d0reez</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Oily face whenever I do nails</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d0reez/oily_face_whenever_i_do_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1d0rbwa</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Current Set</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cf2js0fnjo2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1d0r0n6</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Don’t like this shape for my fingers.</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3iuyoh8bgo2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1d0qzvp</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>just got my first full set in a while</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dq1tz8o3go2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1d0qu1g</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Some of my favorite sets (GelX at home)</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0qu1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1d0ql5e</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Colorful nails 💅🏻🌈</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0ql5e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1d0q7st</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>start the weekend with new nails</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bouiflqx7o2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1d0q466</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Nails for a concert :)</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0q466</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1d0pv92</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>new to this sub, my nail tech 8 these up</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0pv92</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1d0pphi</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Summer Nails!</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0pphi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1d0posl</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Does anyone else experience nail color regret after the salon?</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vajzqrvg2o2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1d0pkxt</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Do these remind you of the 90’s or 80’s at all, or is it just me? 💅😋</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hz19wmgc1o2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1d0pk2v</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">UV nail polish ALWAYS comes off </t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d0pk2v/uv_nail_polish_always_comes_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1d0pe7k</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>First time doing 3d nail art</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/33fi495gzn2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1d0p7k1</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>I think I finally figured out nail foils! I’m absolutely loving layered over chrome look!</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0p7k1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1d0p76i</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dial forms/gel extensions </t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d0p76i/dial_formsgel_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1d0p72k</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>What I decided 😍</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s14rjikhxn2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1d0oy18</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh gel manicure </t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0oy18</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1d0ogs9</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Need Help!! Chrome Art Nails</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d0ogs9/need_help_chrome_art_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1d0o9uc</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>First time for BIAB……</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e83ith5qon2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1d0o8nu</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i love pistachio green! </t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pcafz32fon2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1d0o7hx</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Gel nails lift and peel after 2 days</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7aheksb4on2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1d0o4v4</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Current set 🦋</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/va6wc6bfnn2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1d0nugd</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3rd acrylic set ever! </t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0nugd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1d0nnro</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Which shape do you prefer?</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0nnro</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1d0niap</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Is this blue or green? 🩵💚</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0niap</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1d0nf8u</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why do I keep getting this elevation at the top of my nails. Did I paint them too thick? </t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7mcnfvuygn2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1d0nb7x</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Thought i should include mine &lt;3</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0nb7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1d0n78f</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>MomoCon pressons</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/57gxsg1zen2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1d0mzmy</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Generic title + OC work</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0mzmy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1d0mxkj</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Nail shape? Which suits me best - square-coffin or pointed</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0mxkj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1d0mtwj</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first ILNP order: Charmed and Mutagen...and I got a sticker! </t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jg9t5jsnbn2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1d0moyy</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Blue chrome tips 🩵</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0moyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1d0m8bd</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer nails </t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ns91gozi6n2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1d0m2nx</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Vintage floral mani 🌹</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hdsyxi265n2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1d0lypc</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>I am not a nail art/polish person, but I want to stop picking at my nails so bad, what should I do?</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d0lypc/i_am_not_a_nail_artpolish_person_but_i_want_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1d0lnar</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Killed it, simple bday nails!!</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ptr9tqoe1n2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1d0lera</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Simple but pretty</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0lera</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1d0l1sj</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>💅🏼💙 in love</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q3x2yjy9wm2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1d0kyfy</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9svonlchvm2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1d0ktw9</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Talk me into keeping it!</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1jbdzoydum2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1d0krhg</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>tips on nail art?</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0krhg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1d0kn0b</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Chrome opal nails</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0kn0b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1d0k330</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>🌈</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n9xml95xnm2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1d0jn0l</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Pool Nails 🏊‍♀️</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72xj4fd3km2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1d0j51k</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Something nude again 💅🏻🍂</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0j51k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1d0j2gx</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>I love using mismatched nail stickers :)</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0j2gx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1d0iukq</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Question about nail wraps</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d0iukq/question_about_nail_wraps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1d0ir5x</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>claws🤍</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0ir5x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1d0ig90</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>My black and cheetah set</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0ig90</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1d0ifsp</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>what do you think of these? ☀️</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vnduo0dz9m2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1d0i9xp</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Safety nails </t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xjtwmdn8m2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1d0i04m</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>How do they look?</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ht5wbpzd6m2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1d0hsj0</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Strawberry Milk Tech Redo</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0hsj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1d0hrug</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did some press ons for my sister </t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0hrug</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1d0hd99</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>New manicure</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0hd99</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1d0h5ki</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Set by me on me! </t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0h5ki</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1d0gxx3</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Random designs 👁️💓👑</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0gxx3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1d0gqca</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>I gave myself a manicure!</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0gqca</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1d0gijw</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>My nails that I made myself</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/15i35k1wtl2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1d0gdv8</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>How do y’all get gems/other nail art things to stick on?</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d0gdv8/how_do_yall_get_gemsother_nail_art_things_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1d0g96d</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>I asked for POINTY and she delivered!</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lfcgeuworl2d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1d0fpve</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>DIY 9</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7t4zk1h5nl2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1d0fov7</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Nude nail rec</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0fov7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1d0fkdg</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glittery nails </t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/zBlXEga</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1d0eymm</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Leapord Print nails</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7t0ptwyogl2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1d0evqb</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>First Time Gel at Home!</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0evqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1d0evp2</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Keeping it simple</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gm65r4f0gl2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1d0eshj</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>New set for the weekend 🥰🖤</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3fsd1bp4fl2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1d0erf9</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Got this done and I love it</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngsp150zel2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1d0ep4o</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>I missed my stop bc I was too busy looking at them</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ilm7sgufel2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1d0een2</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How can I make my nails stronger? </t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d0een2/how_can_i_make_my_nails_stronger/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1d0eanx</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>My daughter hooked me up</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0eanx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1d0ea6y</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>New nails! Gotta love a fresh set! 🔮✨💖</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vlmvgidual2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1d0e4hl</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Should I go back to Almond?</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0e4hl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1d0dzhk</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>6 dollar press ons!</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0dzhk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1d0dum1</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>My mom did this set on herself 💅💜</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxtzgp277l2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1d0dlq5</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>I am a beginner and I was thinking of painting press-on nails. I accidentally bought extensions as opposed to full-cover tips. Can I cut and file the extensions to be able to use them for the same function? I could buy the correct thing but I want to use what I have now</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d0dlq5/i_am_a_beginner_and_i_was_thinking_of_painting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1d0dldv</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Selfmade nails with the first time dual tips</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0dldv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1d0dh09</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Feeling blue 💙🩵</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ceo6nqdv3l2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1d0d0wa</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Gel x brand Recs</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d0d0wa/gel_x_brand_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1d0cxjp</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Milky white all the way! 😍</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0cxjp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1d0cns3</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I loooooove long french nails </t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0cns3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1d0cflk</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Soft Gel</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rjtotvyluk2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1d0ca17</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>My nail tech outdid herself</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3azn6et7tk2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1d0c1fz</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My bad </t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sjomtx10rk2d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1d0bpmq</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Sometimes press on nails from the drug store just hit</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpbxdl9xnk2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1d0vq1o</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Nude but fancy</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0vq1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1d0um4n</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Glowy stars</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0um4n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1d0ugiu</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Finally tried this glitter for the first time 🥰🥰</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x3abljhqip2d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1d0ucvl</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>They're different, I swear! (ILNP, Beaux Reves, BKL - Blue + Peach Shimmers)</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0ucvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1d0tu4i</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Beaux Reves - We Are All Made of Stars feat. Mooncat’s Millenia</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0tu4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1d0tq3g</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Reusing masks as nail polish remover cloths</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sbw332d3ap2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1d0tlxh</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I feel like I have jewels on my fingers. </t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0tlxh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1d0sw7q</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>some recent nail looks</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0sw7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1d0sh4j</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>new nail Saturday!! love how these look on my totally natural completely unposed hands 😍</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0sh4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1d0sejz</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help finding an Essie polish I used to have. </t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d0sejz/help_finding_an_essie_polish_i_used_to_have/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1d0ri8b</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>What Would you Do?</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfmisefilo2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1d0qwgl</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Found the perfect mossy polish!</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0qwgl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1d0qm7s</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Cirque Colors- True Love’s First Kiss</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0qm7s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1d0qk7q</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Does anyone know what Mooncat shade this is?</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f9uqvy8ibo2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1d0plti</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Added dry drops instead of polish thinner... How screwed am I?</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d0plti/added_dry_drops_instead_of_polish_thinner_how/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1d0pg1y</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Bruise Purple French Thermals</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0pg1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1d0p1mp</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Holo taco Crushed Holo vs ILNP Ultra Holo?</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d0p1mp/holo_taco_crushed_holo_vs_ilnp_ultra_holo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1d0ooz9</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>When a color looks pretty angled towards the light and straight up fungal against the light</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0ooz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1d0n4ad</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Orange thermals?</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d0n4ad/orange_thermals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1d0mybc</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Dupes for Nailpollies I'm Soy Over It?</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d0mybc/dupes_for_nailpollies_im_soy_over_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1d0mt2q</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>What kind of polish is a good toe polish?</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d0mt2q/what_kind_of_polish_is_a_good_toe_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1d0mri4</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Glitter &amp; green. 💚</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wb66cjg2bn2d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1d0mgdg</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>New fave magnetic</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0mgdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1d0mb14</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Someone here suggested matte top coat on top of jellies 🩵💜💛💚🧡</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0mb14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1d0m32a</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Glitter Polish + Shimmer Topper = Perfection</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xahtlnd95n2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1d0lrhv</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Had to buy both from PPU</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9ql24f9d2n2d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1d0lme3</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Matchy matchy 💜👾🪻</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0lme3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1d0lhd0</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Can’t decide if I like matte or glossy better 🖤🤍 (swipe to see with glossy topcoat!)</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0lhd0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1d0lh2q</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Could I apply either a regular clear topcoat or a cured gel topcoat to my gel mani to extend?</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d0lh2q/could_i_apply_either_a_regular_clear_topcoat_or_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1d0lbno</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Mooncat swatches!</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0lbno</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1d0la2w</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Another week another dotticure</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0la2w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1d0keue</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Custom polish based on a photo?!!!</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0keue</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1d0k3uu</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Saturday mani</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u03yd2b3om2d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1d0k04p</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>🌈Rainbow Streak🌈</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0k04p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1d0jgbn</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>My take on Mondrian art</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0jgbn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1d0j5c2</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>What are the best nail polish formulas for nail art?</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d0j5c2/what_are_the_best_nail_polish_formulas_for_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1d0irh2</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>I spent SO much time on this</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0irh2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1d0inq5</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Is anyone else getting kinda bored with Holo Taco?</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d0inq5/is_anyone_else_getting_kinda_bored_with_holo_taco/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1d0hg90</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>I'm enchanted by Treachery in the Blue</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjbsg1gu1m2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1d0fvfh</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Dust to Dust sponged</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/385i25rgol2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1d0foj9</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>What does your polish storage set up look like?</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d0foj9/what_does_your_polish_storage_set_up_look_like/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1d0f7xo</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Like the night sky ⭐️🌙✨</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0f7xo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1d0ehha</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Replacement caps for Mooncat</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d0ehha/replacement_caps_for_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1d0dr6d</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>I am a beginner and I was thinking of painting press-ons. I accidentally bought extensions as opposed to full-cover tips. Can I cut and file the extensions to be able to use them for the same function, or are they built too differently? I could buy the correct thing but I want to use what I have now</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d0dr6d/i_am_a_beginner_and_i_was_thinking_of_painting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1d0dqoq</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Mooncat Mermaid Bait topped with ILNP Lovebird</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0dqoq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1d0dp4w</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>ILNP Flower Child topped with Mooncat Foxfire</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0dp4w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1d0ct9q</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>How to grow nails again after years of biting</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9o6z76axxk2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1d0c7p5</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Is it safe for a person with intramedullary rod to do magnetic nail art?</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d0c7p5/is_it_safe_for_a_person_with_intramedullary_rod/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1d0bupc</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Such a fun polish!</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljccnq58pk2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1d07p2b</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Help I cant stop buying!</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d07p2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1d07i60</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Have any of you accidentally added something "bad" to your polish?</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d07i60/have_any_of_you_accidentally_added_something_bad/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1d0wi27</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>omg, my boyfriend just said this is the prettiest set of nails I've ever gotten! 💅🏻💖</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0wi27</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1d0v577</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>5 hour set🥲🌺</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wes2r3ferp2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1d0nv3r</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>What do you think of my work!?</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0nv3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1d0mq3x</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>The Nails Bae Gold Chrome Set. IG@NailsByTim6</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwjauocqan2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1d0kzua</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Ocean Nails</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0kzua</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1d0k92c</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Swipe for flash ⚡️</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0k92c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1d0gqkp</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Love this nails</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0gqkp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1d0c4c3</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Hard gel full set with 3D art!</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/amhimmfqrk2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1d0c2e2</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>My bad</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ab7v39j8rk2d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1d0ataw</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Press on of the day</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d0ataw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1d07rbj</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>What do you think of these press ons I made?</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbbpqo90ej2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1d07hgz</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Does anyone else make them so long like this? I love</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2j2zbu1aaj2d1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>